<commit_message>
Adjust groupings (only specimen) and plots
</commit_message>
<xml_diff>
--- a/derived_data/DMTAsharks_EAVP_100x.xlsx
+++ b/derived_data/DMTAsharks_EAVP_100x.xlsx
@@ -15,10 +15,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
-    <t xml:space="preserve">Species</t>
+    <t xml:space="preserve">Specimen</t>
   </si>
   <si>
-    <t xml:space="preserve">Specimen</t>
+    <t xml:space="preserve">Tooth</t>
   </si>
   <si>
     <t xml:space="preserve">Location</t>

</xml_diff>